<commit_message>
reflecting changed plate layout in xlsx : simplified with single delimiter : `_`
</commit_message>
<xml_diff>
--- a/excel files/Plate layouts.xlsx
+++ b/excel files/Plate layouts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
   <si>
     <t xml:space="preserve">C1 should be filled</t>
   </si>
@@ -28,66 +28,255 @@
     <t xml:space="preserve">titles and junk</t>
   </si>
   <si>
+    <t xml:space="preserve">18/Nov/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q40d_S050_fresh transformation_-ves_memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 ul reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qPCRbio probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template type =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasmids + Lysate, LB culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labelling helper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't use "_" in assay variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula helper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target/primer pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assay variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replicate # (optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label_final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formula (add '=')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_miniprep_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_lysate_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ntc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_ntc_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter addition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR(code(T219) + 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-gfp-/103_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gfp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_89.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_miniprep_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_lysate_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_ntc_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter and number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR(code(R341) + 1) &amp; "." &amp; 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-gfptest/186_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_295.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_miniprep_147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_lysate_147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_ntc_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-gfp+/89_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_297.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_colony_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_ntc_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU64/295_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_298.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_colony_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU1/297_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_299.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_colony_147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MG1655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_MG1655_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU8/298_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_300.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triplex_negative_ntc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pPK148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_pPK148_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU34/299_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old16sU64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pPK150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triplex_Control_pPK150_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU73/300_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old16sU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed the labelling format above this</t>
+  </si>
+  <si>
     <t xml:space="preserve">q34_testing template</t>
   </si>
   <si>
-    <t xml:space="preserve">ul template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 ul reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rxn total</t>
-  </si>
-  <si>
     <t xml:space="preserve">qPCRBIO SyGreen 1-Step Detect</t>
   </si>
   <si>
-    <t xml:space="preserve">Template type =</t>
-  </si>
-  <si>
     <t xml:space="preserve">DNAsed RNA extract</t>
   </si>
   <si>
-    <t xml:space="preserve">Labelling helper</t>
-  </si>
-  <si>
     <t xml:space="preserve">Don't use "-",".","_" in assay variable</t>
   </si>
   <si>
-    <t xml:space="preserve">Formula helper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target/primer pair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assay variable</t>
-  </si>
-  <si>
     <t xml:space="preserve">Replicate #</t>
   </si>
   <si>
-    <t xml:space="preserve">Label_final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formula (add '=')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">U64-negative_103.1</t>
   </si>
   <si>
@@ -106,24 +295,6 @@
     <t xml:space="preserve">103</t>
   </si>
   <si>
-    <t xml:space="preserve">Letter addition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR(code(T219) + 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pos-gfp-/103_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gfp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_89.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
     <t xml:space="preserve">U64-negative_ntc.1</t>
   </si>
   <si>
@@ -136,27 +307,6 @@
     <t xml:space="preserve">16s-negative_103.2</t>
   </si>
   <si>
-    <t xml:space="preserve">ntc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Letter and number </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR(code(R341) + 1) &amp; "." &amp; 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pos-gfptest/186_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_295.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
     <t xml:space="preserve">U64-negative_ntc.2</t>
   </si>
   <si>
@@ -169,18 +319,6 @@
     <t xml:space="preserve">16s-positive_295.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-gfp+/89_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_297.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
     <t xml:space="preserve">U64-positive_295.2</t>
   </si>
   <si>
@@ -193,18 +331,6 @@
     <t xml:space="preserve">gfpbarcode</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU64/295_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_298.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
     <t xml:space="preserve">gfpbarcode-negative_ntc.1</t>
   </si>
   <si>
@@ -217,18 +343,6 @@
     <t xml:space="preserve">16s-positive_295.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU1/297_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_299.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
     <t xml:space="preserve">gfpbarcode-negative_ntc.2</t>
   </si>
   <si>
@@ -241,18 +355,6 @@
     <t xml:space="preserve">16s-test_54.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU8/298_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_300.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
     <t xml:space="preserve">U64-test_54.2</t>
   </si>
   <si>
@@ -265,15 +367,6 @@
     <t xml:space="preserve">16s</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU34/299_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">old16sU64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
     <t xml:space="preserve">16s-negative_ntc.2</t>
   </si>
   <si>
@@ -284,24 +377,17 @@
   </si>
   <si>
     <t xml:space="preserve">16s-test_54.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pos-16sU73/300_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">old16sU1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/MMM/YY"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-    <numFmt numFmtId="167" formatCode="D\/MMM\/YY"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="D\/MMM\/YY"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -409,7 +495,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +518,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -546,7 +638,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -583,7 +675,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,7 +711,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,7 +771,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,7 +779,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -703,11 +795,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -715,7 +807,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,7 +815,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,8 +835,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -801,7 +897,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -828,15 +924,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG12"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,56 +978,55 @@
       <c r="AG1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>44734</v>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="9" t="n">
-        <f aca="false">96 - COUNTBLANK(C4:N11)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O2" s="13"/>
       <c r="P2" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="14"/>
       <c r="R2" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S2" s="16"/>
       <c r="T2" s="13"/>
       <c r="U2" s="10"/>
       <c r="V2" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
@@ -942,23 +1040,19 @@
       <c r="AF2" s="13"/>
       <c r="AG2" s="13"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18"/>
       <c r="B3" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="20" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="20" t="n">
-        <v>7</v>
-      </c>
-      <c r="F3" s="20" t="n">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -969,27 +1063,27 @@
       <c r="N3" s="20"/>
       <c r="O3" s="21"/>
       <c r="P3" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T3" s="24"/>
       <c r="U3" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V3" s="25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W3" s="25"/>
       <c r="X3" s="26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
@@ -1001,23 +1095,19 @@
       <c r="AF3" s="13"/>
       <c r="AG3" s="13"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -1040,131 +1130,116 @@
         <v>1</v>
       </c>
       <c r="T4" s="13"/>
-      <c r="U4" s="35" t="str">
-        <f aca="false">P4&amp;"-"&amp;Q4&amp;"_"&amp;R4&amp;"."&amp;S4</f>
-        <v>U64-negative_103.1</v>
+      <c r="U4" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="V4" s="26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W4" s="26"/>
       <c r="X4" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC4" s="13"/>
       <c r="AD4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AF4" s="13"/>
       <c r="AG4" s="13"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="27"/>
       <c r="B5" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="N5" s="38"/>
       <c r="O5" s="21"/>
-      <c r="P5" s="13" t="str">
-        <f aca="false">P4</f>
-        <v>U64</v>
-      </c>
-      <c r="Q5" s="39" t="str">
-        <f aca="false">Q4</f>
-        <v>negative</v>
+      <c r="P5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T5" s="13"/>
+      <c r="U5" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="S5" s="41" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="42" t="str">
-        <f aca="false">P5&amp;"-"&amp;Q5&amp;"_"&amp;R5&amp;"."&amp;S5</f>
-        <v>U64-negative_ntc.1</v>
-      </c>
-      <c r="V5" s="26" t="s">
-        <v>39</v>
       </c>
       <c r="W5" s="26"/>
       <c r="X5" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y5" s="16"/>
       <c r="Z5" s="13"/>
       <c r="AA5" s="13"/>
       <c r="AB5" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC5" s="13"/>
       <c r="AD5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE5" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="AE5" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="AF5" s="13"/>
       <c r="AG5" s="13"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27"/>
       <c r="B6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="D6" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="N6" s="38"/>
       <c r="O6" s="21"/>
-      <c r="P6" s="13" t="str">
-        <f aca="false">P5</f>
-        <v>U64</v>
-      </c>
-      <c r="Q6" s="39" t="str">
-        <f aca="false">Q5</f>
-        <v>negative</v>
+      <c r="P6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="S6" s="41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T6" s="13"/>
-      <c r="U6" s="44" t="str">
-        <f aca="false">P6&amp;"-"&amp;Q6&amp;"_"&amp;R6&amp;"."&amp;S6</f>
-        <v>U64-negative_ntc.2</v>
+      <c r="U6" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="V6" s="13"/>
       <c r="W6" s="13"/>
@@ -1173,54 +1248,48 @@
       <c r="Z6" s="13"/>
       <c r="AA6" s="13"/>
       <c r="AB6" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AC6" s="13"/>
       <c r="AD6" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AE6" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AF6" s="13"/>
       <c r="AG6" s="13"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27"/>
       <c r="B7" s="28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>55</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="N7" s="38"/>
       <c r="O7" s="21"/>
       <c r="P7" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="39" t="str">
-        <f aca="false">Q6</f>
-        <v>negative</v>
+        <v>25</v>
+      </c>
+      <c r="Q7" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R7" s="40" t="s">
         <v>27</v>
       </c>
       <c r="S7" s="41" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T7" s="13"/>
-      <c r="U7" s="44" t="str">
-        <f aca="false">P7&amp;"-"&amp;Q7&amp;"_"&amp;R7&amp;"."&amp;S7</f>
-        <v>gfpbarcode-negative_103.1</v>
+      <c r="U7" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="V7" s="13"/>
       <c r="W7" s="13"/>
@@ -1229,55 +1298,48 @@
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
       <c r="AB7" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AC7" s="13"/>
       <c r="AD7" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AE7" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AF7" s="13"/>
       <c r="AG7" s="13"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27"/>
       <c r="B8" s="28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>64</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="N8" s="38"/>
       <c r="O8" s="21"/>
-      <c r="P8" s="13" t="str">
-        <f aca="false">P7</f>
-        <v>gfpbarcode</v>
-      </c>
-      <c r="Q8" s="39" t="str">
-        <f aca="false">Q7</f>
-        <v>negative</v>
+      <c r="P8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="S8" s="41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8" s="13"/>
-      <c r="U8" s="44" t="str">
-        <f aca="false">P8&amp;"-"&amp;Q8&amp;"_"&amp;R8&amp;"."&amp;S8</f>
-        <v>gfpbarcode-negative_ntc.1</v>
+      <c r="U8" s="44" t="s">
+        <v>37</v>
       </c>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
@@ -1286,55 +1348,48 @@
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="26" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AC8" s="13"/>
       <c r="AD8" s="13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="AF8" s="13"/>
       <c r="AG8" s="13"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27"/>
       <c r="B9" s="28" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>72</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
-      <c r="P9" s="13" t="str">
-        <f aca="false">P8</f>
-        <v>gfpbarcode</v>
-      </c>
-      <c r="Q9" s="39" t="str">
-        <f aca="false">Q8</f>
-        <v>negative</v>
+      <c r="P9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="S9" s="41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T9" s="13"/>
-      <c r="U9" s="44" t="str">
-        <f aca="false">P9&amp;"-"&amp;Q9&amp;"_"&amp;R9&amp;"."&amp;S9</f>
-        <v>gfpbarcode-negative_ntc.2</v>
+      <c r="U9" s="44" t="s">
+        <v>64</v>
       </c>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
@@ -1343,54 +1398,48 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
       <c r="AB9" s="26" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="AC9" s="13"/>
       <c r="AD9" s="13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="AE9" s="13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="AF9" s="13"/>
       <c r="AG9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27"/>
       <c r="B10" s="28" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>79</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="N10" s="38"/>
       <c r="O10" s="21"/>
       <c r="P10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q10" s="39" t="str">
-        <f aca="false">Q9</f>
-        <v>negative</v>
+        <v>25</v>
+      </c>
+      <c r="Q10" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="S10" s="41" t="n">
         <v>1</v>
       </c>
       <c r="T10" s="13"/>
-      <c r="U10" s="44" t="str">
-        <f aca="false">P10&amp;"-"&amp;Q10&amp;"_"&amp;R10&amp;"."&amp;S10</f>
-        <v>16s-negative_103.1</v>
+      <c r="U10" s="44" t="s">
+        <v>71</v>
       </c>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
@@ -1399,35 +1448,31 @@
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
       <c r="AB10" s="26" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="AC10" s="13"/>
       <c r="AD10" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AF10" s="13"/>
       <c r="AG10" s="13"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="45"/>
       <c r="B11" s="19" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>87</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -1437,24 +1482,21 @@
       <c r="M11" s="47"/>
       <c r="N11" s="48"/>
       <c r="O11" s="21"/>
-      <c r="P11" s="13" t="str">
-        <f aca="false">P10</f>
-        <v>16s</v>
-      </c>
-      <c r="Q11" s="39" t="str">
-        <f aca="false">Q10</f>
-        <v>negative</v>
+      <c r="P11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="S11" s="41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11" s="13"/>
-      <c r="U11" s="49" t="str">
-        <f aca="false">P11&amp;"-"&amp;Q11&amp;"_"&amp;R11&amp;"."&amp;S11</f>
-        <v>16s-negative_ntc.2</v>
+      <c r="U11" s="49" t="s">
+        <v>76</v>
       </c>
       <c r="V11" s="13"/>
       <c r="W11" s="13"/>
@@ -1463,30 +1505,634 @@
       <c r="Z11" s="13"/>
       <c r="AA11" s="13"/>
       <c r="AB11" s="26" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AC11" s="13"/>
       <c r="AD11" s="16" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AE11" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AF11" s="13"/>
       <c r="AG11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="50"/>
-      <c r="C12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="R12" s="37"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>44734</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="9" t="n">
+        <f aca="false">96 - COUNTBLANK(C15:N22)</f>
+        <v>32</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="O13" s="13"/>
+      <c r="P13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="S13" s="16"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" s="20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F14" s="20" t="n">
+        <v>9</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="S14" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="T14" s="24"/>
+      <c r="U14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V14" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="W14" s="25"/>
+      <c r="X14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="13"/>
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q15" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="R15" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="S15" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" s="13"/>
+      <c r="U15" s="35" t="str">
+        <f aca="false">P15&amp;"-"&amp;Q15&amp;"_"&amp;R15&amp;"."&amp;S15</f>
+        <v>U64-negative_103.1</v>
+      </c>
+      <c r="V15" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="W15" s="26"/>
+      <c r="X15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF15" s="13"/>
+      <c r="AG15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="N16" s="38"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="13" t="str">
+        <f aca="false">P15</f>
+        <v>U64</v>
+      </c>
+      <c r="Q16" s="39" t="str">
+        <f aca="false">Q15</f>
+        <v>negative</v>
+      </c>
+      <c r="R16" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T16" s="13"/>
+      <c r="U16" s="42" t="str">
+        <f aca="false">P16&amp;"-"&amp;Q16&amp;"_"&amp;R16&amp;"."&amp;S16</f>
+        <v>U64-negative_ntc.1</v>
+      </c>
+      <c r="V16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="W16" s="26"/>
+      <c r="X16" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF16" s="13"/>
+      <c r="AG16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="N17" s="38"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="13" t="str">
+        <f aca="false">P16</f>
+        <v>U64</v>
+      </c>
+      <c r="Q17" s="39" t="str">
+        <f aca="false">Q16</f>
+        <v>negative</v>
+      </c>
+      <c r="R17" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T17" s="13"/>
+      <c r="U17" s="44" t="str">
+        <f aca="false">P17&amp;"-"&amp;Q17&amp;"_"&amp;R17&amp;"."&amp;S17</f>
+        <v>U64-negative_ntc.2</v>
+      </c>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE17" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" s="38"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q18" s="39" t="str">
+        <f aca="false">Q17</f>
+        <v>negative</v>
+      </c>
+      <c r="R18" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="S18" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" s="13"/>
+      <c r="U18" s="44" t="str">
+        <f aca="false">P18&amp;"-"&amp;Q18&amp;"_"&amp;R18&amp;"."&amp;S18</f>
+        <v>gfpbarcode-negative_103.1</v>
+      </c>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC18" s="13"/>
+      <c r="AD18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE18" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF18" s="13"/>
+      <c r="AG18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A19" s="27"/>
+      <c r="B19" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="N19" s="38"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="13" t="str">
+        <f aca="false">P18</f>
+        <v>gfpbarcode</v>
+      </c>
+      <c r="Q19" s="39" t="str">
+        <f aca="false">Q18</f>
+        <v>negative</v>
+      </c>
+      <c r="R19" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="S19" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T19" s="13"/>
+      <c r="U19" s="44" t="str">
+        <f aca="false">P19&amp;"-"&amp;Q19&amp;"_"&amp;R19&amp;"."&amp;S19</f>
+        <v>gfpbarcode-negative_ntc.1</v>
+      </c>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="13" t="str">
+        <f aca="false">P19</f>
+        <v>gfpbarcode</v>
+      </c>
+      <c r="Q20" s="39" t="str">
+        <f aca="false">Q19</f>
+        <v>negative</v>
+      </c>
+      <c r="R20" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="S20" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T20" s="13"/>
+      <c r="U20" s="44" t="str">
+        <f aca="false">P20&amp;"-"&amp;Q20&amp;"_"&amp;R20&amp;"."&amp;S20</f>
+        <v>gfpbarcode-negative_ntc.2</v>
+      </c>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC20" s="13"/>
+      <c r="AD20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF20" s="13"/>
+      <c r="AG20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A21" s="27"/>
+      <c r="B21" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="N21" s="38"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q21" s="39" t="str">
+        <f aca="false">Q20</f>
+        <v>negative</v>
+      </c>
+      <c r="R21" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="S21" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" s="13"/>
+      <c r="U21" s="44" t="str">
+        <f aca="false">P21&amp;"-"&amp;Q21&amp;"_"&amp;R21&amp;"."&amp;S21</f>
+        <v>16s-negative_103.1</v>
+      </c>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A22" s="45"/>
+      <c r="B22" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="13" t="str">
+        <f aca="false">P21</f>
+        <v>16s</v>
+      </c>
+      <c r="Q22" s="39" t="str">
+        <f aca="false">Q21</f>
+        <v>negative</v>
+      </c>
+      <c r="R22" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T22" s="13"/>
+      <c r="U22" s="49" t="str">
+        <f aca="false">P22&amp;"-"&amp;Q22&amp;"_"&amp;R22&amp;"."&amp;S22</f>
+        <v>16s-negative_ntc.2</v>
+      </c>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF22" s="13"/>
+      <c r="AG22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="51"/>
+      <c r="C23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="R23" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Z3"/>
@@ -1495,6 +2141,14 @@
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="X6:Y6"/>
     <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="X18:Y18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
more updates to README and updated Plate layout with current example q50 data
</commit_message>
<xml_diff>
--- a/excel files/Plate layouts.xlsx
+++ b/excel files/Plate layouts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="154">
   <si>
     <t xml:space="preserve">C1 should be filled</t>
   </si>
@@ -28,69 +28,273 @@
     <t xml:space="preserve">titles and junk</t>
   </si>
   <si>
+    <t xml:space="preserve">27/May/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q50_S080-RAM repression 80a, mjd61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 ul reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qPCRbio probe 1-step Go + qPCRBIO Sygreen Blue mix (not meant for RT) + qPCRbio RT mix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template type =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNAsed RNA extract / 10x dil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labelling helper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't use "_" in assay variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula helper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target/primer pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assay variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replicate # (optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label_final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formula (add '=')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRP name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_negative_MG1655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_Repressed_MJD61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_Maximal_AOS107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_negative_MG1655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_Repressed_MJD61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_Maximal_AOS107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter addition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR(code(T219) + 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-gfp-/103_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gfp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_89.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_Maximal_80a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_Maximal_80a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter and number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR(code(R341) + 1) &amp; "." &amp; 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-gfptest/186_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_295.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-gfp+/89_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_297.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No mastermix :(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_Maximal_MJD61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_Maximal_AOS109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_Maximal_MJD61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_Maximal_AOS109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU64/295_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_298.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_Repressed_80a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_Repressed_80a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU1/297_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_299.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU8/298_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16sU73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_300.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU34/299_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old16sU64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplex_negative_NTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_negative_NTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_V2-3_1e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos-16sU73/300_1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old16sU1</t>
+  </si>
+  <si>
     <t xml:space="preserve">18/Nov/22</t>
   </si>
   <si>
     <t xml:space="preserve">q40d_S050_fresh transformation_-ves_memory</t>
   </si>
   <si>
-    <t xml:space="preserve">ul template</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 ul reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rxn total</t>
-  </si>
-  <si>
     <t xml:space="preserve">qPCRbio probe</t>
   </si>
   <si>
-    <t xml:space="preserve">Template type =</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plasmids + Lysate, LB culture</t>
   </si>
   <si>
-    <t xml:space="preserve">Labelling helper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don't use "_" in assay variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formula helper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target/primer pair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assay variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replicate # (optional)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label_final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formula (add '=')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_miniprep_143</t>
   </si>
   <si>
@@ -109,24 +313,6 @@
     <t xml:space="preserve">Triplex_Control_ntc_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Letter addition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR(code(T219) + 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pos-gfp-/103_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gfp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_89.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_miniprep_144</t>
   </si>
   <si>
@@ -136,24 +322,6 @@
     <t xml:space="preserve">Triplex_Control_ntc_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Letter and number </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR(code(R341) + 1) &amp; "." &amp; 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pos-gfptest/186_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_295.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_miniprep_147</t>
   </si>
   <si>
@@ -163,51 +331,15 @@
     <t xml:space="preserve">Triplex_Control_ntc_3</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-gfp+/89_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_297.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_colony_143</t>
   </si>
   <si>
     <t xml:space="preserve">Triplex_Control_ntc_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU64/295_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_298.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_colony_144</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU1/297_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_299.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_colony_147</t>
   </si>
   <si>
@@ -217,18 +349,6 @@
     <t xml:space="preserve">Triplex_Control_MG1655_3</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU8/298_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16sU73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test_300.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
     <t xml:space="preserve">triplex_negative_ntc</t>
   </si>
   <si>
@@ -238,25 +358,10 @@
     <t xml:space="preserve">Triplex_Control_pPK148_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Pos-16sU34/299_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">old16sU64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
     <t xml:space="preserve">pPK150</t>
   </si>
   <si>
     <t xml:space="preserve">Triplex_Control_pPK150_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pos-16sU73/300_1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">old16sU1</t>
   </si>
   <si>
     <t xml:space="preserve">Changed the labelling format above this</t>
@@ -638,7 +743,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,8 +924,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -837,6 +942,10 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -924,7 +1033,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
@@ -934,7 +1043,7 @@
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -998,7 +1107,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="9" t="n">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>7</v>
@@ -1049,12 +1158,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
@@ -1096,20 +1213,30 @@
       <c r="AG3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27"/>
+      <c r="A4" s="27" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -1118,128 +1245,150 @@
       <c r="N4" s="31"/>
       <c r="O4" s="21"/>
       <c r="P4" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="34" t="n">
-        <v>1</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="R4" s="33" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="S4" s="34"/>
       <c r="T4" s="13"/>
       <c r="U4" s="35" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="V4" s="26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="W4" s="26"/>
       <c r="X4" s="16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AC4" s="13"/>
       <c r="AD4" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AF4" s="13"/>
       <c r="AG4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27"/>
+      <c r="A5" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="B5" s="28" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="N5" s="38"/>
       <c r="O5" s="21"/>
       <c r="P5" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="40" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="R5" s="40" t="n">
+        <v>10000000</v>
       </c>
       <c r="S5" s="41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T5" s="13"/>
       <c r="U5" s="42" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="W5" s="26"/>
       <c r="X5" s="43" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="Y5" s="16"/>
       <c r="Z5" s="13"/>
       <c r="AA5" s="13"/>
       <c r="AB5" s="26" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="AC5" s="13"/>
       <c r="AD5" s="13" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="AE5" s="13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AF5" s="13"/>
       <c r="AG5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27"/>
+      <c r="A6" s="27" t="s">
+        <v>48</v>
+      </c>
       <c r="B6" s="28" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="N6" s="38"/>
       <c r="O6" s="21"/>
       <c r="P6" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" s="40" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="R6" s="40" t="n">
+        <v>1000000</v>
       </c>
       <c r="S6" s="41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T6" s="13"/>
       <c r="U6" s="44" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="V6" s="13"/>
       <c r="W6" s="13"/>
@@ -1248,48 +1397,60 @@
       <c r="Z6" s="13"/>
       <c r="AA6" s="13"/>
       <c r="AB6" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="AC6" s="13"/>
       <c r="AD6" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="AE6" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AF6" s="13"/>
       <c r="AG6" s="13"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="s">
+        <v>54</v>
+      </c>
       <c r="B7" s="28" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="N7" s="38"/>
       <c r="O7" s="21"/>
       <c r="P7" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R7" s="40" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="R7" s="40" t="n">
+        <v>100000</v>
       </c>
       <c r="S7" s="41" t="n">
         <v>4</v>
       </c>
       <c r="T7" s="13"/>
       <c r="U7" s="44" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="V7" s="13"/>
       <c r="W7" s="13"/>
@@ -1298,48 +1459,58 @@
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
       <c r="AB7" s="26" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AC7" s="13"/>
       <c r="AD7" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="AE7" s="13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="AF7" s="13"/>
       <c r="AG7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="N8" s="38"/>
       <c r="O8" s="21"/>
       <c r="P8" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="40" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="R8" s="40" t="n">
+        <v>10000</v>
       </c>
       <c r="S8" s="41" t="n">
         <v>2</v>
       </c>
       <c r="T8" s="13"/>
       <c r="U8" s="44" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
@@ -1348,48 +1519,58 @@
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="26" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AC8" s="13"/>
       <c r="AD8" s="13" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AF8" s="13"/>
       <c r="AG8" s="13"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="s">
+        <v>57</v>
+      </c>
       <c r="B9" s="28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="P9" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="40" t="s">
-        <v>63</v>
+        <v>31</v>
+      </c>
+      <c r="R9" s="40" t="n">
+        <v>1000</v>
       </c>
       <c r="S9" s="41" t="n">
         <v>3</v>
       </c>
       <c r="T9" s="13"/>
       <c r="U9" s="44" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
@@ -1398,48 +1579,53 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
       <c r="AB9" s="26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AC9" s="13"/>
       <c r="AD9" s="13" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AE9" s="13" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AF9" s="13"/>
       <c r="AG9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="28" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>66</v>
+      </c>
       <c r="N10" s="38"/>
       <c r="O10" s="21"/>
       <c r="P10" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="40" t="s">
-        <v>70</v>
+        <v>31</v>
+      </c>
+      <c r="R10" s="40" t="n">
+        <v>100</v>
       </c>
       <c r="S10" s="41" t="n">
         <v>1</v>
       </c>
       <c r="T10" s="13"/>
       <c r="U10" s="44" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
@@ -1448,14 +1634,14 @@
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
       <c r="AB10" s="26" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AC10" s="13"/>
       <c r="AD10" s="13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AF10" s="13"/>
       <c r="AG10" s="13"/>
@@ -1463,17 +1649,21 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="45"/>
       <c r="B11" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
@@ -1483,20 +1673,20 @@
       <c r="N11" s="48"/>
       <c r="O11" s="21"/>
       <c r="P11" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R11" s="40" t="s">
-        <v>75</v>
+        <v>31</v>
+      </c>
+      <c r="R11" s="40" t="n">
+        <v>10</v>
       </c>
       <c r="S11" s="41" t="n">
         <v>1</v>
       </c>
       <c r="T11" s="13"/>
       <c r="U11" s="49" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="V11" s="13"/>
       <c r="W11" s="13"/>
@@ -1505,32 +1695,60 @@
       <c r="Z11" s="13"/>
       <c r="AA11" s="13"/>
       <c r="AB11" s="26" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="AC11" s="13"/>
       <c r="AD11" s="16" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AE11" s="16" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AF11" s="13"/>
       <c r="AG11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
-        <v>44734</v>
+      <c r="A13" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D13" s="7" t="n">
         <v>4</v>
@@ -1539,28 +1757,27 @@
         <v>4</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="9" t="n">
-        <f aca="false">96 - COUNTBLANK(C15:N22)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="11" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="O13" s="13"/>
       <c r="P13" s="14" t="s">
@@ -1568,7 +1785,7 @@
       </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="15" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="S13" s="16"/>
       <c r="T13" s="13"/>
@@ -1588,7 +1805,7 @@
       <c r="AF13" s="13"/>
       <c r="AG13" s="13"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
         <v>14</v>
@@ -1597,14 +1814,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E14" s="20" t="n">
-        <v>7</v>
-      </c>
-      <c r="F14" s="20" t="n">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -1624,7 +1837,7 @@
         <v>17</v>
       </c>
       <c r="S14" s="24" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="T14" s="24"/>
       <c r="U14" s="17" t="s">
@@ -1647,23 +1860,19 @@
       <c r="AF14" s="13"/>
       <c r="AG14" s="13"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
       <c r="B15" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -1674,143 +1883,128 @@
       <c r="N15" s="31"/>
       <c r="O15" s="21"/>
       <c r="P15" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="Q15" s="32" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="R15" s="33" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="S15" s="34" t="n">
         <v>1</v>
       </c>
       <c r="T15" s="13"/>
-      <c r="U15" s="35" t="str">
-        <f aca="false">P15&amp;"-"&amp;Q15&amp;"_"&amp;R15&amp;"."&amp;S15</f>
-        <v>U64-negative_103.1</v>
+      <c r="U15" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="V15" s="26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="W15" s="26"/>
       <c r="X15" s="16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Y15" s="16"/>
       <c r="Z15" s="16"/>
       <c r="AA15" s="13"/>
       <c r="AB15" s="13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AC15" s="13"/>
       <c r="AD15" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AF15" s="13"/>
       <c r="AG15" s="13"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27"/>
       <c r="B16" s="28" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>94</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
       <c r="N16" s="38"/>
       <c r="O16" s="21"/>
-      <c r="P16" s="13" t="str">
-        <f aca="false">P15</f>
-        <v>U64</v>
-      </c>
-      <c r="Q16" s="39" t="str">
-        <f aca="false">Q15</f>
-        <v>negative</v>
+      <c r="P16" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q16" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R16" s="40" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="S16" s="41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T16" s="13"/>
-      <c r="U16" s="42" t="str">
-        <f aca="false">P16&amp;"-"&amp;Q16&amp;"_"&amp;R16&amp;"."&amp;S16</f>
-        <v>U64-negative_ntc.1</v>
+      <c r="U16" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="V16" s="26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="W16" s="26"/>
       <c r="X16" s="43" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="Y16" s="16"/>
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
       <c r="AB16" s="26" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="AC16" s="13"/>
       <c r="AD16" s="13" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="AE16" s="13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AF16" s="13"/>
       <c r="AG16" s="13"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>98</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
       <c r="N17" s="38"/>
       <c r="O17" s="21"/>
-      <c r="P17" s="13" t="str">
-        <f aca="false">P16</f>
-        <v>U64</v>
-      </c>
-      <c r="Q17" s="39" t="str">
-        <f aca="false">Q16</f>
-        <v>negative</v>
+      <c r="P17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R17" s="40" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="S17" s="41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T17" s="13"/>
-      <c r="U17" s="44" t="str">
-        <f aca="false">P17&amp;"-"&amp;Q17&amp;"_"&amp;R17&amp;"."&amp;S17</f>
-        <v>U64-negative_ntc.2</v>
+      <c r="U17" s="44" t="s">
+        <v>102</v>
       </c>
       <c r="V17" s="13"/>
       <c r="W17" s="13"/>
@@ -1819,54 +2013,48 @@
       <c r="Z17" s="13"/>
       <c r="AA17" s="13"/>
       <c r="AB17" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="AC17" s="13"/>
       <c r="AD17" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="AE17" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AF17" s="13"/>
       <c r="AG17" s="13"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27"/>
       <c r="B18" s="28" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>101</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
       <c r="N18" s="38"/>
       <c r="O18" s="21"/>
       <c r="P18" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q18" s="39" t="str">
-        <f aca="false">Q17</f>
-        <v>negative</v>
+        <v>93</v>
+      </c>
+      <c r="Q18" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R18" s="40" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="S18" s="41" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T18" s="13"/>
-      <c r="U18" s="44" t="str">
-        <f aca="false">P18&amp;"-"&amp;Q18&amp;"_"&amp;R18&amp;"."&amp;S18</f>
-        <v>gfpbarcode-negative_103.1</v>
+      <c r="U18" s="44" t="s">
+        <v>104</v>
       </c>
       <c r="V18" s="13"/>
       <c r="W18" s="13"/>
@@ -1875,55 +2063,48 @@
       <c r="Z18" s="13"/>
       <c r="AA18" s="13"/>
       <c r="AB18" s="26" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AC18" s="13"/>
       <c r="AD18" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="AE18" s="13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="AF18" s="13"/>
       <c r="AG18" s="13"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="27"/>
       <c r="B19" s="28" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>106</v>
-      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
       <c r="N19" s="38"/>
       <c r="O19" s="21"/>
-      <c r="P19" s="13" t="str">
-        <f aca="false">P18</f>
-        <v>gfpbarcode</v>
-      </c>
-      <c r="Q19" s="39" t="str">
-        <f aca="false">Q18</f>
-        <v>negative</v>
+      <c r="P19" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q19" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R19" s="40" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="S19" s="41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T19" s="13"/>
-      <c r="U19" s="44" t="str">
-        <f aca="false">P19&amp;"-"&amp;Q19&amp;"_"&amp;R19&amp;"."&amp;S19</f>
-        <v>gfpbarcode-negative_ntc.1</v>
+      <c r="U19" s="44" t="s">
+        <v>99</v>
       </c>
       <c r="V19" s="13"/>
       <c r="W19" s="13"/>
@@ -1932,55 +2113,48 @@
       <c r="Z19" s="13"/>
       <c r="AA19" s="13"/>
       <c r="AB19" s="26" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AC19" s="13"/>
       <c r="AD19" s="13" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="AE19" s="13" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AF19" s="13"/>
       <c r="AG19" s="13"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27"/>
       <c r="B20" s="28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>110</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
-      <c r="P20" s="13" t="str">
-        <f aca="false">P19</f>
-        <v>gfpbarcode</v>
-      </c>
-      <c r="Q20" s="39" t="str">
-        <f aca="false">Q19</f>
-        <v>negative</v>
+      <c r="P20" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q20" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R20" s="40" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="S20" s="41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T20" s="13"/>
-      <c r="U20" s="44" t="str">
-        <f aca="false">P20&amp;"-"&amp;Q20&amp;"_"&amp;R20&amp;"."&amp;S20</f>
-        <v>gfpbarcode-negative_ntc.2</v>
+      <c r="U20" s="44" t="s">
+        <v>108</v>
       </c>
       <c r="V20" s="13"/>
       <c r="W20" s="13"/>
@@ -1989,54 +2163,48 @@
       <c r="Z20" s="13"/>
       <c r="AA20" s="13"/>
       <c r="AB20" s="26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AC20" s="13"/>
       <c r="AD20" s="13" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AE20" s="13" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AF20" s="13"/>
       <c r="AG20" s="13"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27"/>
       <c r="B21" s="28" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>113</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
       <c r="N21" s="38"/>
       <c r="O21" s="21"/>
       <c r="P21" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q21" s="39" t="str">
-        <f aca="false">Q20</f>
-        <v>negative</v>
+        <v>93</v>
+      </c>
+      <c r="Q21" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R21" s="40" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="S21" s="41" t="n">
         <v>1</v>
       </c>
       <c r="T21" s="13"/>
-      <c r="U21" s="44" t="str">
-        <f aca="false">P21&amp;"-"&amp;Q21&amp;"_"&amp;R21&amp;"."&amp;S21</f>
-        <v>16s-negative_103.1</v>
+      <c r="U21" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="V21" s="13"/>
       <c r="W21" s="13"/>
@@ -2045,35 +2213,31 @@
       <c r="Z21" s="13"/>
       <c r="AA21" s="13"/>
       <c r="AB21" s="26" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AC21" s="13"/>
       <c r="AD21" s="13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AE21" s="13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AF21" s="13"/>
       <c r="AG21" s="13"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A22" s="45"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="50"/>
       <c r="B22" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D22" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>118</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -2083,24 +2247,21 @@
       <c r="M22" s="47"/>
       <c r="N22" s="48"/>
       <c r="O22" s="21"/>
-      <c r="P22" s="13" t="str">
-        <f aca="false">P21</f>
-        <v>16s</v>
-      </c>
-      <c r="Q22" s="39" t="str">
-        <f aca="false">Q21</f>
-        <v>negative</v>
+      <c r="P22" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q22" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="R22" s="40" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="S22" s="41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T22" s="13"/>
-      <c r="U22" s="49" t="str">
-        <f aca="false">P22&amp;"-"&amp;Q22&amp;"_"&amp;R22&amp;"."&amp;S22</f>
-        <v>16s-negative_ntc.2</v>
+      <c r="U22" s="49" t="s">
+        <v>113</v>
       </c>
       <c r="V22" s="13"/>
       <c r="W22" s="13"/>
@@ -2109,30 +2270,634 @@
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
       <c r="AB22" s="26" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="AC22" s="13"/>
       <c r="AD22" s="16" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AE22" s="16" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AF22" s="13"/>
       <c r="AG22" s="13"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="51"/>
-      <c r="C23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="R23" s="37"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
+        <v>44734</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="9" t="n">
+        <f aca="false">96 - COUNTBLANK(C26:N33)</f>
+        <v>32</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24" s="13"/>
+      <c r="P24" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="S24" s="16"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
+      <c r="AF24" s="13"/>
+      <c r="AG24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" s="20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F25" s="20" t="n">
+        <v>9</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q25" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R25" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="S25" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="T25" s="24"/>
+      <c r="U25" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V25" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="W25" s="25"/>
+      <c r="X25" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="13"/>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A26" s="27"/>
+      <c r="B26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q26" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="R26" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="S26" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="T26" s="13"/>
+      <c r="U26" s="35" t="str">
+        <f aca="false">P26&amp;"-"&amp;Q26&amp;"_"&amp;R26&amp;"."&amp;S26</f>
+        <v>U64-negative_103.1</v>
+      </c>
+      <c r="V26" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="W26" s="26"/>
+      <c r="X26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF26" s="13"/>
+      <c r="AG26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A27" s="27"/>
+      <c r="B27" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="N27" s="38"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="13" t="str">
+        <f aca="false">P26</f>
+        <v>U64</v>
+      </c>
+      <c r="Q27" s="39" t="str">
+        <f aca="false">Q26</f>
+        <v>negative</v>
+      </c>
+      <c r="R27" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="S27" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T27" s="13"/>
+      <c r="U27" s="42" t="str">
+        <f aca="false">P27&amp;"-"&amp;Q27&amp;"_"&amp;R27&amp;"."&amp;S27</f>
+        <v>U64-negative_ntc.1</v>
+      </c>
+      <c r="V27" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="W27" s="26"/>
+      <c r="X27" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC27" s="13"/>
+      <c r="AD27" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE27" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A28" s="27"/>
+      <c r="B28" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="N28" s="38"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="13" t="str">
+        <f aca="false">P27</f>
+        <v>U64</v>
+      </c>
+      <c r="Q28" s="39" t="str">
+        <f aca="false">Q27</f>
+        <v>negative</v>
+      </c>
+      <c r="R28" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="S28" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T28" s="13"/>
+      <c r="U28" s="44" t="str">
+        <f aca="false">P28&amp;"-"&amp;Q28&amp;"_"&amp;R28&amp;"."&amp;S28</f>
+        <v>U64-negative_ntc.2</v>
+      </c>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="13"/>
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC28" s="13"/>
+      <c r="AD28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE28" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="13"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A29" s="27"/>
+      <c r="B29" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="N29" s="38"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q29" s="39" t="str">
+        <f aca="false">Q28</f>
+        <v>negative</v>
+      </c>
+      <c r="R29" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S29" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T29" s="13"/>
+      <c r="U29" s="44" t="str">
+        <f aca="false">P29&amp;"-"&amp;Q29&amp;"_"&amp;R29&amp;"."&amp;S29</f>
+        <v>gfpbarcode-negative_103.1</v>
+      </c>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE29" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A30" s="27"/>
+      <c r="B30" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="N30" s="38"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="13" t="str">
+        <f aca="false">P29</f>
+        <v>gfpbarcode</v>
+      </c>
+      <c r="Q30" s="39" t="str">
+        <f aca="false">Q29</f>
+        <v>negative</v>
+      </c>
+      <c r="R30" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="S30" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T30" s="13"/>
+      <c r="U30" s="44" t="str">
+        <f aca="false">P30&amp;"-"&amp;Q30&amp;"_"&amp;R30&amp;"."&amp;S30</f>
+        <v>gfpbarcode-negative_ntc.1</v>
+      </c>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC30" s="13"/>
+      <c r="AD30" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE30" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="13"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A31" s="27"/>
+      <c r="B31" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="13" t="str">
+        <f aca="false">P30</f>
+        <v>gfpbarcode</v>
+      </c>
+      <c r="Q31" s="39" t="str">
+        <f aca="false">Q30</f>
+        <v>negative</v>
+      </c>
+      <c r="R31" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="S31" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T31" s="13"/>
+      <c r="U31" s="44" t="str">
+        <f aca="false">P31&amp;"-"&amp;Q31&amp;"_"&amp;R31&amp;"."&amp;S31</f>
+        <v>gfpbarcode-negative_ntc.2</v>
+      </c>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC31" s="13"/>
+      <c r="AD31" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE31" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A32" s="27"/>
+      <c r="B32" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="N32" s="38"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q32" s="39" t="str">
+        <f aca="false">Q31</f>
+        <v>negative</v>
+      </c>
+      <c r="R32" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S32" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T32" s="13"/>
+      <c r="U32" s="44" t="str">
+        <f aca="false">P32&amp;"-"&amp;Q32&amp;"_"&amp;R32&amp;"."&amp;S32</f>
+        <v>16s-negative_103.1</v>
+      </c>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE32" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF32" s="13"/>
+      <c r="AG32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A33" s="50"/>
+      <c r="B33" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="13" t="str">
+        <f aca="false">P32</f>
+        <v>16s</v>
+      </c>
+      <c r="Q33" s="39" t="str">
+        <f aca="false">Q32</f>
+        <v>negative</v>
+      </c>
+      <c r="R33" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="S33" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="T33" s="13"/>
+      <c r="U33" s="49" t="str">
+        <f aca="false">P33&amp;"-"&amp;Q33&amp;"_"&amp;R33&amp;"."&amp;S33</f>
+        <v>16s-negative_ntc.2</v>
+      </c>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC33" s="13"/>
+      <c r="AD33" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="52"/>
+      <c r="C34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="R34" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="26">
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Z3"/>
@@ -2140,7 +2905,9 @@
     <mergeCell ref="X4:Z4"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="X14:Z14"/>
@@ -2149,6 +2916,14 @@
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="X17:Y17"/>
     <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Z25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="X26:Z26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="X29:Y29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>